<commit_message>
Add Save In 1 Word File + optimize
</commit_message>
<xml_diff>
--- a/DbFolder/ParkingDB.xlsx
+++ b/DbFolder/ParkingDB.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="521">
   <si>
     <t>Id</t>
   </si>
@@ -1582,6 +1582,12 @@
   </si>
   <si>
     <t>335ea5a2-436d-4ff6-8556-fca100072d8c</t>
+  </si>
+  <si>
+    <t>eb33ae18-ac75-4f14-98b9-3ba6accf121d</t>
+  </si>
+  <si>
+    <t>27.01.2025 21:43:37</t>
   </si>
 </sst>
 </file>
@@ -3140,7 +3146,7 @@
         <v>207</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33">
@@ -4953,7 +4959,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
@@ -5070,6 +5076,41 @@
         <v>500</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="H4" s="0">
+        <v>31</v>
+      </c>
+      <c r="I4" s="0">
+        <v>213</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>486</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
fix validate XAML + backend
</commit_message>
<xml_diff>
--- a/DbFolder/ParkingDB.xlsx
+++ b/DbFolder/ParkingDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepositories\parkingWPF_project\DbFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A149233E-48ED-4F48-A838-5FEDBA51EDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C025E8-B19C-4855-91B6-0E03A311C030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Owners" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <sheet name="Vehicles" sheetId="5" r:id="rId5"/>
     <sheet name="Receipts" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" fullPrecision="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="522">
   <si>
     <t>Id</t>
   </si>
@@ -1020,7 +1020,7 @@
     <t>734299ee-1cf1-4138-8112-4d49ea1d6aaf</t>
   </si>
   <si>
-    <t>c2c49830-68a9-4c01-bd7d-d6f7bea9cf10</t>
+    <t>e3d91ac9-0ba5-483d-adef-74d40cc0dcec</t>
   </si>
   <si>
     <t>528a7b0d-42f4-48de-b4e7-991ae9838f8d</t>
@@ -1170,7 +1170,7 @@
     <t>205771db-176b-4079-8235-49b097534790</t>
   </si>
   <si>
-    <t>Е 456 КХ 92</t>
+    <t>Е456КХ92</t>
   </si>
   <si>
     <t>Micro</t>
@@ -1182,7 +1182,7 @@
     <t>f59d3fdd-7cc7-4875-b1b8-c7b568bea727</t>
   </si>
   <si>
-    <t>О 056 НМ 43</t>
+    <t>О056НМ43</t>
   </si>
   <si>
     <t>Bentley</t>
@@ -1194,7 +1194,7 @@
     <t>dd9e784e-c37a-4781-8e13-7e2569421720</t>
   </si>
   <si>
-    <t>Х 242 ЕВ 09</t>
+    <t>Х242ЕВ09</t>
   </si>
   <si>
     <t>Maserati</t>
@@ -1206,7 +1206,7 @@
     <t>b70f5a3f-61c4-4461-ae10-04b071559f4a</t>
   </si>
   <si>
-    <t>К 169 МХ 65</t>
+    <t>К169МХ65</t>
   </si>
   <si>
     <t>Hyundai</t>
@@ -1218,7 +1218,7 @@
     <t>4cb4c663-50d7-4973-a222-44e7a5fc3e6d</t>
   </si>
   <si>
-    <t>Р 567 АВ 85</t>
+    <t>Р567АВ85</t>
   </si>
   <si>
     <t>Citroen</t>
@@ -1230,7 +1230,7 @@
     <t>7d80bbae-b546-4b1c-bf3f-833b5452a884</t>
   </si>
   <si>
-    <t>М 286 КО 05</t>
+    <t>М286КО05</t>
   </si>
   <si>
     <t>Tucson</t>
@@ -1239,7 +1239,7 @@
     <t>ab13c5d2-4d8e-41d1-a554-8fe2ab7db098</t>
   </si>
   <si>
-    <t>Т 624 СН 21</t>
+    <t>Т624СН21</t>
   </si>
   <si>
     <t>Toyota</t>
@@ -1251,7 +1251,7 @@
     <t>6db56ce2-078a-411a-a29f-95769c3765d1</t>
   </si>
   <si>
-    <t>Е 388 НМ 33</t>
+    <t>Е388НМ33</t>
   </si>
   <si>
     <t>Subaru</t>
@@ -1263,7 +1263,7 @@
     <t>6f4058d9-8157-4364-a9da-edbb271ba7b7</t>
   </si>
   <si>
-    <t>А 277 ЕУ 23</t>
+    <t>А277ЕУ23</t>
   </si>
   <si>
     <t>Ford</t>
@@ -1275,7 +1275,7 @@
     <t>95182947-67d5-4eaa-8255-38534656e70c</t>
   </si>
   <si>
-    <t>О 791 ЕН 164</t>
+    <t>О791ЕН164</t>
   </si>
   <si>
     <t>Vauxhall</t>
@@ -1287,7 +1287,7 @@
     <t>625e9b95-74c5-47f6-84c0-efd23428c37f</t>
   </si>
   <si>
-    <t>О 315 ХХ 04</t>
+    <t>О315ХХ04</t>
   </si>
   <si>
     <t>Morgan</t>
@@ -1299,7 +1299,7 @@
     <t>865dd671-7cf2-494c-bd2c-e6e77c8ae26e</t>
   </si>
   <si>
-    <t>А 908 МЕ 777</t>
+    <t>А908МЕ777</t>
   </si>
   <si>
     <t>LeBlanc</t>
@@ -1311,7 +1311,7 @@
     <t>9bcff96f-d8b3-4944-86d3-ba1d3db4e39f</t>
   </si>
   <si>
-    <t>У 642 ОМ 27</t>
+    <t>У642ОМ27</t>
   </si>
   <si>
     <t>Plus Six</t>
@@ -1320,7 +1320,7 @@
     <t>de247204-d7d9-4343-a8df-af345da82fa1</t>
   </si>
   <si>
-    <t>О 342 НР 43</t>
+    <t>О342НР43</t>
   </si>
   <si>
     <t>Lotus</t>
@@ -1332,7 +1332,7 @@
     <t>baac1806-5667-4d53-be64-099fcc6f7a1e</t>
   </si>
   <si>
-    <t>К 331 СС 40</t>
+    <t>К331СС40</t>
   </si>
   <si>
     <t>Nissan</t>
@@ -1344,7 +1344,7 @@
     <t>7b753bc7-2886-42d2-ba62-5dd571d78e14</t>
   </si>
   <si>
-    <t>В 852 РВ 14</t>
+    <t>В852РВ14</t>
   </si>
   <si>
     <t>SsangYong</t>
@@ -1356,7 +1356,7 @@
     <t>2a54c2a3-83f5-4575-9a16-73f284b3374f</t>
   </si>
   <si>
-    <t>У 696 ТУ 59</t>
+    <t>У696ТУ59</t>
   </si>
   <si>
     <t>Rolls-Royce</t>
@@ -1368,7 +1368,7 @@
     <t>17395c9c-586b-464c-bcf9-e7461f6ebe08</t>
   </si>
   <si>
-    <t>Т 429 МЕ 87</t>
+    <t>Т429МЕ87</t>
   </si>
   <si>
     <t>Camry</t>
@@ -1377,7 +1377,7 @@
     <t>fdaaa3f4-5c5e-4372-9427-9baade575a33</t>
   </si>
   <si>
-    <t>К 198 УО 43</t>
+    <t>К198УО43</t>
   </si>
   <si>
     <t>Suzuki</t>
@@ -1389,7 +1389,7 @@
     <t>aa364b1e-ef31-41ca-bd40-3f5e591976d8</t>
   </si>
   <si>
-    <t>Р 397 РА 763</t>
+    <t>Р397РА763</t>
   </si>
   <si>
     <t>Lifan</t>
@@ -1401,7 +1401,7 @@
     <t>5d323ced-98d2-4fdf-af59-631cfdc5c19f</t>
   </si>
   <si>
-    <t>А 045 ЕР 17</t>
+    <t>А045ЕР17</t>
   </si>
   <si>
     <t>DS</t>
@@ -1413,7 +1413,7 @@
     <t>e14eb2f1-4dfa-4a7e-bece-d8389159d4e3</t>
   </si>
   <si>
-    <t>С 715 ЕС 142</t>
+    <t>С715ЕС142</t>
   </si>
   <si>
     <t>Mazda</t>
@@ -1425,7 +1425,7 @@
     <t>035c963d-a69b-4139-ba71-89bbb0286843</t>
   </si>
   <si>
-    <t>М 909 НУ 44</t>
+    <t>М909НУ44</t>
   </si>
   <si>
     <t>F-150</t>
@@ -1434,7 +1434,7 @@
     <t>c782f415-5dfa-4914-909a-57f80547172a</t>
   </si>
   <si>
-    <t>Х 264 МЕ 50</t>
+    <t>Х264МЕ50</t>
   </si>
   <si>
     <t>Corsa</t>
@@ -1443,7 +1443,7 @@
     <t>8ddd90f6-57cc-4a54-8bc0-45e28fdd062b</t>
   </si>
   <si>
-    <t>А 060 РЕ 12</t>
+    <t>А060РЕ12</t>
   </si>
   <si>
     <t>Laraki</t>
@@ -1455,7 +1455,7 @@
     <t>1681c7c0-d64e-4383-8d05-be559ffee6a2</t>
   </si>
   <si>
-    <t>Н 309 МА 31</t>
+    <t>Н309МА31</t>
   </si>
   <si>
     <t>Honda</t>
@@ -1467,7 +1467,7 @@
     <t>3de9aaf8-d8dd-44b7-9cf1-4022a8ed1abf</t>
   </si>
   <si>
-    <t>Е 535 ОС 116</t>
+    <t>Е535ОС116</t>
   </si>
   <si>
     <t>Mitsubishi</t>
@@ -1479,7 +1479,7 @@
     <t>c6f96d79-2737-4d81-8493-10e0ebd654c0</t>
   </si>
   <si>
-    <t>Е 778 УЕ 76</t>
+    <t>Е778УЕ76</t>
   </si>
   <si>
     <t>Lancia</t>
@@ -1491,7 +1491,7 @@
     <t>fb1569f5-9baf-472b-bdc5-811071cfd701</t>
   </si>
   <si>
-    <t>К 474 НК 725</t>
+    <t>К474НК725</t>
   </si>
   <si>
     <t>C3</t>
@@ -1500,7 +1500,7 @@
     <t>ba38ca46-50bb-43ca-a070-4c38c84ad16b</t>
   </si>
   <si>
-    <t>Н 562 КС 754</t>
+    <t>Н562КС754</t>
   </si>
   <si>
     <t>McLaren</t>
@@ -1512,7 +1512,7 @@
     <t>7fc22324-d5ee-4a7d-89cf-25d7e114ef80</t>
   </si>
   <si>
-    <t>М 730 ВУ 774</t>
+    <t>M730BY774</t>
   </si>
   <si>
     <t>Lada</t>
@@ -1524,7 +1524,7 @@
     <t>bf989544-ff5f-45d9-8275-73cdd9a25f8a</t>
   </si>
   <si>
-    <t>К 548 СК 174</t>
+    <t>K548CK174</t>
   </si>
   <si>
     <t>2109</t>
@@ -1533,7 +1533,7 @@
     <t>42da13c2-cb72-4538-92c8-9d29ec318bb6</t>
   </si>
   <si>
-    <t>Е 666 КХ 777</t>
+    <t>Е666КХ777</t>
   </si>
   <si>
     <t>BMW</t>
@@ -1597,7 +1597,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1941,672 +1942,673 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="5">
+      <c r="A5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="6">
+      <c r="A6" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="0" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="7">
+      <c r="A7" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="0" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="8">
+      <c r="A8" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="0" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="9">
+      <c r="A9" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="0" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="10">
+      <c r="A10" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="0" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="11">
+      <c r="A11" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="0" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="12">
+      <c r="A12" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="0" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="13">
+      <c r="A13" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="0" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+    <row r="14">
+      <c r="A14" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="0" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    <row r="15">
+      <c r="A15" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="0" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+    <row r="16">
+      <c r="A16" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="0" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+    <row r="17">
+      <c r="A17" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="0" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+    <row r="18">
+      <c r="A18" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="0" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="19">
+      <c r="A19" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+    <row r="20">
+      <c r="A20" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="0" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+    <row r="21">
+      <c r="A21" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="0" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+    <row r="22">
+      <c r="A22" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="0" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+    <row r="23">
+      <c r="A23" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="0" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+    <row r="24">
+      <c r="A24" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="0" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="25">
+      <c r="A25" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="0" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+    <row r="26">
+      <c r="A26" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="0" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="27">
+      <c r="A27" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="0" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+    <row r="28">
+      <c r="A28" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="0" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="29">
+      <c r="A29" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="0" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+    <row r="30">
+      <c r="A30" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="0" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+    <row r="31">
+      <c r="A31" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="0" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+    <row r="32">
+      <c r="A32" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="0" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+    <row r="33">
+      <c r="A33" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="0" t="s">
         <v>187</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -2614,89 +2616,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="A6:D8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="2" max="2" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.796875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="5">
+      <c r="A5" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>204</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -2704,1328 +2700,1334 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D100" sqref="A94:D100"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" bestFit="1" width="10.46484375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="D3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="D3" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="D4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="D4" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="D5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="D5" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="D6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="D6" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="D7" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="D7" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="D8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="D8" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="D9" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="D9" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="D10" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="D10" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="D11" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+      <c r="D11" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="D12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="D12" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="D13" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="D13" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="D14" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="D14" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="D15" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="D15" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="D16" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+      <c r="D16" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="D17" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+      <c r="D17" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="D18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+      <c r="D18" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="D19" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+      <c r="D19" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="D20" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+      <c r="D20" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="D21" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+      <c r="D21" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="D22" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+      <c r="D22" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="D23" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+      <c r="D23" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="D24" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+      <c r="D24" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="D25" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+      <c r="D25" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="D26" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+      <c r="D26" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="D27" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+      <c r="D27" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="D28" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+      <c r="D28" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="D29" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+      <c r="D29" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="D30" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+      <c r="D30" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="D31" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+      <c r="D31" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="0" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+    <row r="33">
+      <c r="A33" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="D33" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+      <c r="D33" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="D34" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+      <c r="D34" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="D35" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
+      <c r="D35" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="D36" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+      <c r="D36" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="s">
         <v>274</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="D37" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
+      <c r="D37" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="D38" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+      <c r="D38" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="D39" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+      <c r="D39" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="D40" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+      <c r="D40" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="D41" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
+      <c r="D41" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="D42" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+      <c r="D42" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="D43" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
+      <c r="D43" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="D44" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
+      <c r="D44" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="D45" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
+      <c r="D45" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="s">
         <v>283</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="D46" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+      <c r="D46" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="D47" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
+      <c r="D47" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="D48" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
+      <c r="D48" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="D49" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+      <c r="D49" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="s">
         <v>287</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="D50" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+      <c r="D50" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="D51" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+      <c r="D51" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="D52" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+      <c r="D52" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="D53" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+      <c r="D53" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="D54" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
+      <c r="D54" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="D55" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+      <c r="D55" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="D56" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
+      <c r="D56" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="D57" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
+      <c r="D57" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="D58" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
+      <c r="D58" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0" t="s">
         <v>296</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="D59" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
+      <c r="D59" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="D60" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+      <c r="D60" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0" t="s">
         <v>298</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="D61" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
+      <c r="D61" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="D62" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
+      <c r="D62" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0" t="s">
         <v>300</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="D63" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
+      <c r="D63" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0" t="s">
         <v>301</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="D64" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
+      <c r="D64" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="D65" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
+      <c r="D65" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="D66" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
+      <c r="D66" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0" t="s">
         <v>304</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="D67" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
+      <c r="D67" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="D68" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
+      <c r="D68" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0" t="s">
         <v>306</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="D69" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
+      <c r="D69" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0" t="s">
         <v>307</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="D70" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
+      <c r="D70" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="0" t="s">
         <v>308</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="D71" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
+      <c r="D71" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0" t="s">
         <v>309</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="D72" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
+      <c r="D72" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="D73" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
+      <c r="D73" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="0" t="s">
         <v>311</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="D74" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
+      <c r="D74" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="0" t="s">
         <v>312</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="D75" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
+      <c r="D75" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="0" t="s">
         <v>313</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="D76" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
+      <c r="D76" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="0" t="s">
         <v>314</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="D77" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
+      <c r="D77" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="0" t="s">
         <v>315</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="D78" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
+      <c r="D78" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="0" t="s">
         <v>316</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="D79" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
+      <c r="D79" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="0" t="s">
         <v>317</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="D80" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
+      <c r="D80" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="0" t="s">
         <v>318</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="D81" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
+      <c r="D81" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="D82" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A83" t="s">
+      <c r="D82" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="D83" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A84" t="s">
+      <c r="D83" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="0" t="s">
         <v>321</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="D84" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A85" t="s">
+      <c r="D84" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="D85" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A86" t="s">
+      <c r="D85" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="0" t="s">
         <v>323</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="D86" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A87" t="s">
+      <c r="D86" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="D87" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A88" t="s">
+      <c r="D87" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="D88" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A89" t="s">
+      <c r="D88" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="D89" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A90" t="s">
+      <c r="D89" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="D90" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A91" t="s">
+      <c r="D90" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="D91" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A92" t="s">
+      <c r="D91" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="0" t="s">
         <v>329</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="0" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A93" t="s">
+    <row r="93">
+      <c r="A93" s="0" t="s">
         <v>330</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="D93" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A94" t="s">
+      <c r="D93" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="0" t="s">
         <v>331</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="0" t="s">
         <v>212</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -4037,232 +4039,233 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" s="0" t="s">
         <v>332</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>333</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" s="0" t="s">
         <v>335</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" s="0" t="s">
         <v>337</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>339</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="5">
+      <c r="A5" s="0" t="s">
         <v>341</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>342</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>343</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="6">
+      <c r="A6" s="0" t="s">
         <v>345</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>346</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="7">
+      <c r="A7" s="0" t="s">
         <v>347</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>348</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="8">
+      <c r="A8" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>352</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>353</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="0" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="9">
+      <c r="A9" s="0" t="s">
         <v>354</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>355</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="0" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="10">
+      <c r="A10" s="0" t="s">
         <v>357</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>358</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="0" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="11">
+      <c r="A11" s="0" t="s">
         <v>360</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="0" t="s">
         <v>361</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="12">
+      <c r="A12" s="0" t="s">
         <v>362</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>363</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="0" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="13">
+      <c r="A13" s="0" t="s">
         <v>364</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>365</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="0" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+    <row r="14">
+      <c r="A14" s="0" t="s">
         <v>366</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>367</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="0" t="s">
         <v>368</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="0" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    <row r="15">
+      <c r="A15" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>370</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="0" t="s">
         <v>371</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="0" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+    <row r="16">
+      <c r="A16" s="0" t="s">
         <v>372</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>373</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="0" t="s">
         <v>374</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="0" t="s">
         <v>140</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -4270,694 +4273,693 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>375</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>376</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>377</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>378</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>381</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>382</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>383</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" s="0" t="s">
         <v>384</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>385</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>386</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>387</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" s="0" t="s">
         <v>388</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>389</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>390</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>391</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="5">
+      <c r="A5" s="0" t="s">
         <v>392</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>393</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>394</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="0" t="s">
         <v>395</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="6">
+      <c r="A6" s="0" t="s">
         <v>396</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>398</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="7">
+      <c r="A7" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>401</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>394</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="0" t="s">
         <v>402</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="8">
+      <c r="A8" s="0" t="s">
         <v>403</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>404</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="0" t="s">
         <v>405</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="0" t="s">
         <v>406</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="9">
+      <c r="A9" s="0" t="s">
         <v>407</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>408</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="0" t="s">
         <v>409</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="0" t="s">
         <v>410</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="10">
+      <c r="A10" s="0" t="s">
         <v>411</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>412</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="0" t="s">
         <v>413</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="0" t="s">
         <v>414</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="11">
+      <c r="A11" s="0" t="s">
         <v>415</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="0" t="s">
         <v>416</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="0" t="s">
         <v>417</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="0" t="s">
         <v>418</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="12">
+      <c r="A12" s="0" t="s">
         <v>419</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>420</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="0" t="s">
         <v>421</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="0" t="s">
         <v>422</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="0">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="13">
+      <c r="A13" s="0" t="s">
         <v>423</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>424</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="0" t="s">
         <v>425</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="0" t="s">
         <v>426</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+    <row r="14">
+      <c r="A14" s="0" t="s">
         <v>427</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="0" t="s">
         <v>428</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="0" t="s">
         <v>421</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="0" t="s">
         <v>429</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    <row r="15">
+      <c r="A15" s="0" t="s">
         <v>430</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="0" t="s">
         <v>431</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="0" t="s">
         <v>432</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="0" t="s">
         <v>433</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+    <row r="16">
+      <c r="A16" s="0" t="s">
         <v>434</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="0" t="s">
         <v>435</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="0" t="s">
         <v>436</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="0" t="s">
         <v>437</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+    <row r="17">
+      <c r="A17" s="0" t="s">
         <v>438</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="0" t="s">
         <v>439</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="0" t="s">
         <v>440</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="0" t="s">
         <v>441</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+    <row r="18">
+      <c r="A18" s="0" t="s">
         <v>442</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="0" t="s">
         <v>443</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="0" t="s">
         <v>444</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="0" t="s">
         <v>445</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="19">
+      <c r="A19" s="0" t="s">
         <v>446</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="0" t="s">
         <v>447</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="0" t="s">
         <v>405</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="0" t="s">
         <v>448</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+    <row r="20">
+      <c r="A20" s="0" t="s">
         <v>449</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="0" t="s">
         <v>451</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="0" t="s">
         <v>452</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+    <row r="21">
+      <c r="A21" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="0" t="s">
         <v>454</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="0" t="s">
         <v>455</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="0" t="s">
         <v>456</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+    <row r="22">
+      <c r="A22" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="0" t="s">
         <v>458</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="0" t="s">
         <v>459</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="0" t="s">
         <v>460</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="0">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+    <row r="23">
+      <c r="A23" s="0" t="s">
         <v>461</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="0" t="s">
         <v>462</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="0" t="s">
         <v>463</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="0" t="s">
         <v>464</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+    <row r="24">
+      <c r="A24" s="0" t="s">
         <v>465</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="0" t="s">
         <v>413</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="0" t="s">
         <v>467</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="25">
+      <c r="A25" s="0" t="s">
         <v>468</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="0" t="s">
         <v>469</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="0" t="s">
         <v>417</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="0" t="s">
         <v>470</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+    <row r="26">
+      <c r="A26" s="0" t="s">
         <v>471</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="0" t="s">
         <v>472</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="0" t="s">
         <v>473</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="0" t="s">
         <v>474</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="0">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="27">
+      <c r="A27" s="0" t="s">
         <v>475</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="0" t="s">
         <v>476</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="0" t="s">
         <v>477</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="0" t="s">
         <v>478</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="0">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+    <row r="28">
+      <c r="A28" s="0" t="s">
         <v>479</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="0" t="s">
         <v>480</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="0" t="s">
         <v>481</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="0" t="s">
         <v>482</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="29">
+      <c r="A29" s="0" t="s">
         <v>483</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="0" t="s">
         <v>484</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="0" t="s">
         <v>485</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="0" t="s">
         <v>486</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="0">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+    <row r="30">
+      <c r="A30" s="0" t="s">
         <v>487</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="0" t="s">
         <v>488</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="0" t="s">
         <v>398</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="0" t="s">
         <v>489</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="0">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+    <row r="31">
+      <c r="A31" s="0" t="s">
         <v>490</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="0" t="s">
         <v>491</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="0" t="s">
         <v>492</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="0" t="s">
         <v>493</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+    <row r="32">
+      <c r="A32" s="0" t="s">
         <v>494</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="0" t="s">
         <v>495</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="0" t="s">
         <v>496</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="0" t="s">
         <v>497</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+    <row r="33">
+      <c r="A33" s="0" t="s">
         <v>498</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="0" t="s">
         <v>499</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="0" t="s">
         <v>496</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="0" t="s">
         <v>500</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="0">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+    <row r="34">
+      <c r="A34" s="0" t="s">
         <v>501</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="0" t="s">
         <v>502</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="0" t="s">
         <v>503</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="0" t="s">
         <v>504</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="0">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -4965,157 +4967,152 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="10" max="10" width="23.265625" customWidth="1"/>
-    <col min="11" max="11" width="33.59765625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>505</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>506</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>507</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>508</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>509</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>510</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="0" t="s">
         <v>512</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="0" t="s">
         <v>513</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="0" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" s="0" t="s">
         <v>515</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>517</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="0" t="s">
         <v>362</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0">
         <v>31</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>189</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="0" t="s">
         <v>518</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="0" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" s="0" t="s">
         <v>519</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>517</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="0" t="s">
         <v>329</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="0" t="s">
         <v>362</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0">
         <v>30</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0">
         <v>199</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="0" t="s">
         <v>518</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="0" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" s="0" t="s">
         <v>520</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>517</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="0" t="s">
         <v>364</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0">
         <v>31</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>213</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="0" t="s">
         <v>521</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="0" t="s">
         <v>487</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>